<commit_message>
Update books_data.xlsx with latest scraped data
</commit_message>
<xml_diff>
--- a/IntermediateLevel/WebScrapper/books_data.xlsx
+++ b/IntermediateLevel/WebScrapper/books_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Shadowfox-python-internship\IntermediateLevel\Scrapper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Shadowfox-python-internship\IntermediateLevel\WebScrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933F0052-B60C-4439-8B74-CEC2F00392C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD35DB9-3CE0-435D-8B29-3F17DFA09110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>